<commit_message>
Documentação e ajustes finos
</commit_message>
<xml_diff>
--- a/modelagem/UseCaseDescription/DCU0001-ManterPersonagens.xlsx
+++ b/modelagem/UseCaseDescription/DCU0001-ManterPersonagens.xlsx
@@ -105,7 +105,7 @@
     <t>Alterar Personagem</t>
   </si>
   <si>
-    <t>(A2.01) Seleciona o personagens que se deseja alterar</t>
+    <t>(A2.01) Seleciona o personagem que se deseja alterar</t>
   </si>
   <si>
     <t>(A2.02) Clica no botão "Editar" na parte superior da tabela</t>
@@ -727,7 +727,7 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="2"/>

</xml_diff>